<commit_message>
Zähigkeit hinzugefügt, PAP2.1 Heft hinzugefügt
</commit_message>
<xml_diff>
--- a/RLC Glied.xlsx
+++ b/RLC Glied.xlsx
@@ -226,14 +226,14 @@
         <v>0.05</v>
       </c>
       <c r="E4" s="3">
-        <v>0.03</v>
+        <v>0.003</v>
       </c>
       <c r="F4" s="3">
         <v>0.002</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="6"/>
-        <v>0.00004328085123</v>
+        <v>0.000004328085123</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="3"/>

</xml_diff>